<commit_message>
Se reviso y se encontro que se usaron ATB-2020 en el modelo para CT. No se incluyo CC
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_ThermalGEN_NewOilfield.xlsx
+++ b/SubRES_TMPL/SubRES_ThermalGEN_NewOilfield.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Pictures\TIMES-O-G-B\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARMEN\Pictures\ModeloTIMESOG\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71B3894-BCD0-4CED-A059-5164FAB92AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E68E0D5-A2D8-43FB-9339-38705583A7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thermal_MID" sheetId="5" r:id="rId1"/>
@@ -632,11 +632,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -921,7 +921,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="61">
@@ -945,16 +945,16 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1001,8 +1001,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -1012,7 +1012,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1055,7 +1055,7 @@
     <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="3" applyFill="1"/>
@@ -1398,81 +1398,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0ACBD7-08CE-4A0A-8F39-4F100175164B}">
   <dimension ref="A4:W39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="7" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="10" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
-    <col min="15" max="15" width="30.44140625" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" customWidth="1"/>
-    <col min="17" max="17" width="19.77734375" customWidth="1"/>
-    <col min="19" max="19" width="29.109375" customWidth="1"/>
-    <col min="20" max="20" width="12.77734375" customWidth="1"/>
-    <col min="21" max="21" width="18.21875" customWidth="1"/>
-    <col min="22" max="22" width="17.88671875" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
+    <col min="19" max="19" width="29.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" customWidth="1"/>
+    <col min="22" max="22" width="17.85546875" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="57"/>
       <c r="C4" s="58"/>
       <c r="D4" s="58"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="45"/>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
       <c r="D8" s="43"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
       <c r="D9" s="43"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
       <c r="D10" s="43"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
       <c r="D11" s="43"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="43"/>
       <c r="C12" s="43"/>
@@ -1484,7 +1484,7 @@
         <v>75.166375708662926</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="45"/>
       <c r="C13" s="43"/>
@@ -1496,7 +1496,7 @@
         <v>77.841777688967127</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" s="46"/>
       <c r="C14" s="48"/>
@@ -1508,7 +1508,7 @@
         <v>55.539114956987063</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
       <c r="B15" s="49"/>
       <c r="C15" s="47"/>
@@ -1520,13 +1520,13 @@
         <v>78.281203343664757</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
       <c r="B16" s="49"/>
       <c r="C16" s="47"/>
       <c r="D16" s="49"/>
     </row>
-    <row r="18" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:23" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="30"/>
@@ -1549,7 +1549,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="2:23" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:23" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="30"/>
@@ -1572,19 +1572,19 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>1</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
         <v>2</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O16</f>
         <v>AUTOCOL-NE-DSL1-CAM8</v>
@@ -1686,7 +1686,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O17</f>
         <v>AUTOCOL-NE-HFO1-CAM8</v>
@@ -1736,7 +1736,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O18</f>
         <v>AUTOCOL-NE-OIL1-CAM8</v>
@@ -1786,7 +1786,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O19</f>
         <v>AUTOCOL-NE-GASCT1-CAM8</v>
@@ -1836,7 +1836,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O20</f>
         <v>AUTOCOL-NE-GASCT2-CAM8</v>
@@ -1886,7 +1886,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O21</f>
         <v>AUTOCOL-NE-GASCT3-CAM8</v>
@@ -1939,7 +1939,7 @@
       <c r="V30" s="33"/>
       <c r="W30" s="33"/>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1952,7 +1952,7 @@
       <c r="K31" s="53"/>
       <c r="L31" s="43"/>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1965,7 +1965,7 @@
       <c r="K32" s="53"/>
       <c r="L32" s="43"/>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1978,7 +1978,7 @@
       <c r="K33" s="53"/>
       <c r="L33" s="43"/>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1991,7 +1991,7 @@
       <c r="K34" s="53"/>
       <c r="L34" s="43"/>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2004,7 +2004,7 @@
       <c r="K35" s="53"/>
       <c r="L35" s="42"/>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2017,10 +2017,10 @@
       <c r="K36" s="53"/>
       <c r="L36" s="43"/>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="U38" s="23"/>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="U39" s="22"/>
     </row>
   </sheetData>
@@ -2042,48 +2042,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:W39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I26" sqref="B26:I26"/>
+    <sheetView showGridLines="0" topLeftCell="E8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="7" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.21875" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
-    <col min="15" max="15" width="30.44140625" customWidth="1"/>
-    <col min="16" max="16" width="18.21875" customWidth="1"/>
-    <col min="17" max="17" width="19.77734375" customWidth="1"/>
-    <col min="19" max="19" width="29.109375" customWidth="1"/>
-    <col min="20" max="20" width="12.77734375" customWidth="1"/>
-    <col min="21" max="21" width="18.21875" customWidth="1"/>
-    <col min="22" max="22" width="17.88671875" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
+    <col min="19" max="19" width="29.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" customWidth="1"/>
+    <col min="22" max="22" width="17.85546875" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="59" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>50</v>
       </c>
@@ -2110,10 +2110,10 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2124,7 +2124,7 @@
         <v>75.166375708662926</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>77.841777688967127</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>55.539114956987063</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>B9</f>
         <v>FTE-FUEL-OIL-CAM8</v>
@@ -2172,7 +2172,7 @@
         <v>78.281203343664757</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>B10</f>
         <v>FTE-FUEL-GAS-CAM8</v>
@@ -2184,12 +2184,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="30"/>
     </row>
-    <row r="19" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:23" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="30"/>
@@ -2212,7 +2212,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:23" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:23" ht="23.25" x14ac:dyDescent="0.25">
       <c r="I20" s="14" t="s">
         <v>60</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>1</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
         <v>2</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O10</f>
         <v>AUTO-NE-DSL1-CAM8</v>
@@ -2346,7 +2346,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O11</f>
         <v>AUTO-NE-HFO1-CAM8</v>
@@ -2395,7 +2395,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O12</f>
         <v>AUTO-NE-OIL1-CAM8</v>
@@ -2445,7 +2445,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O13</f>
         <v>AUTO-NE-GASCT1-CAM8</v>
@@ -2495,7 +2495,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O14</f>
         <v>AUTO-NE-GASCT2-CAM8</v>
@@ -2545,7 +2545,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="str">
         <f>'COMM&amp;PROCESS'!O15</f>
         <v>AUTO-NE-GASCT3-CAM8</v>
@@ -2598,7 +2598,7 @@
       <c r="V30" s="33"/>
       <c r="W30" s="33"/>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" s="43"/>
       <c r="C31" s="43"/>
       <c r="D31" s="43"/>
@@ -2611,7 +2611,7 @@
       <c r="K31" s="53"/>
       <c r="L31" s="43"/>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="43"/>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
@@ -2624,7 +2624,7 @@
       <c r="K32" s="53"/>
       <c r="L32" s="43"/>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="43"/>
       <c r="C33" s="43"/>
       <c r="D33" s="43"/>
@@ -2637,7 +2637,7 @@
       <c r="K33" s="53"/>
       <c r="L33" s="43"/>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="43"/>
       <c r="C34" s="43"/>
       <c r="D34" s="43"/>
@@ -2650,7 +2650,7 @@
       <c r="K34" s="53"/>
       <c r="L34" s="43"/>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="43"/>
       <c r="C35" s="43"/>
       <c r="D35" s="43"/>
@@ -2663,7 +2663,7 @@
       <c r="K35" s="53"/>
       <c r="L35" s="42"/>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
@@ -2676,10 +2676,10 @@
       <c r="K36" s="53"/>
       <c r="L36" s="43"/>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="U38" s="23"/>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="U39" s="22"/>
     </row>
   </sheetData>
@@ -2706,15 +2706,15 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="36.88671875" customWidth="1"/>
-    <col min="15" max="15" width="31.5546875" customWidth="1"/>
-    <col min="16" max="16" width="44.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="15" max="15" width="31.5703125" customWidth="1"/>
+    <col min="16" max="16" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M4" s="10" t="s">
         <v>9</v>
       </c>
@@ -2727,7 +2727,7 @@
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:21" ht="32.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:21" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
         <v>25</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="T7" s="13"/>
       <c r="U7" s="13"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>41</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D9" s="55" t="str">
         <f>Thermal_UP!C10</f>
         <v>GAS-CAM8</v>
@@ -2919,7 +2919,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D10" t="str">
         <f>Thermal_UP!C15</f>
         <v>FUEL-OIL-CAM8</v>
@@ -2947,7 +2947,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D11" t="str">
         <f>Thermal_UP!C16</f>
         <v>FUEL-GAS-CAM8</v>
@@ -2973,7 +2973,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D12" s="55" t="s">
         <v>48</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D13" s="55" t="s">
         <v>76</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="F14" s="5"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
@@ -3040,7 +3040,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
       <c r="O15" s="34" t="s">
@@ -3056,7 +3056,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
       <c r="O16" s="34" t="s">
@@ -3072,7 +3072,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="13:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
       <c r="O17" s="34" t="s">
@@ -3088,7 +3088,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="13:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
       <c r="O18" s="34" t="s">
@@ -3104,7 +3104,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="13:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M19" s="34"/>
       <c r="N19" s="34"/>
       <c r="O19" s="34" t="s">
@@ -3120,7 +3120,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="13:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M20" s="34"/>
       <c r="N20" s="34"/>
       <c r="O20" s="34" t="s">
@@ -3136,7 +3136,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="13:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M21" s="34"/>
       <c r="N21" s="34"/>
       <c r="O21" s="34" t="s">

</xml_diff>